<commit_message>
Made a figure of the measured blue and red MOT coils. I should make a theory plot if I have time.
</commit_message>
<xml_diff>
--- a/chapters/experiment/mot_coils/Rydberg-MOTCoilFieldMeasurement.xlsx
+++ b/chapters/experiment/mot_coils/Rydberg-MOTCoilFieldMeasurement.xlsx
@@ -1,21 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyalp\Documents\GitHub\phd_thesis\chapters\experiment\mot_coils\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028E9D72-D778-4A87-BC44-0943538B137D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="19815" windowHeight="11445" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlueMOTCoil" sheetId="3" r:id="rId1"/>
     <sheet name="RedMOTCoil" sheetId="1" r:id="rId2"/>
+    <sheet name="Data-BlueCoil1" sheetId="6" r:id="rId3"/>
+    <sheet name="Data-BlueCoil2" sheetId="7" r:id="rId4"/>
+    <sheet name="Data-BlueMOTCoil" sheetId="4" r:id="rId5"/>
+    <sheet name="Data-RedCoil1" sheetId="8" r:id="rId6"/>
+    <sheet name="Data-RedCoil2" sheetId="9" r:id="rId7"/>
+    <sheet name="Data-RedMOTCoil" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>Red Mot Coils Test</t>
   </si>
@@ -118,11 +138,23 @@
   <si>
     <t>4A*10</t>
   </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>B_z</t>
+  </si>
+  <si>
+    <t>B_y</t>
+  </si>
+  <si>
+    <t>B_x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -179,12 +211,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -213,7 +248,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -334,6 +368,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BCD-4010-A45C-F8D17DB91607}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -447,6 +486,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9BCD-4010-A45C-F8D17DB91607}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -575,6 +619,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9BCD-4010-A45C-F8D17DB91607}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -610,7 +659,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -644,7 +692,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -684,7 +731,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -698,7 +745,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -818,6 +864,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3557-4080-BA9C-D59A261B8951}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -853,7 +904,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -887,7 +937,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -913,7 +962,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1061,6 +1110,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E795-4614-90BE-4340DD8596D9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1209,7 +1263,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1238,7 +1292,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1359,6 +1412,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28B8-4B7F-AE0D-18BA46B90362}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1472,6 +1530,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-28B8-4B7F-AE0D-18BA46B90362}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1600,6 +1663,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-28B8-4B7F-AE0D-18BA46B90362}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1635,7 +1703,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1669,7 +1736,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1709,7 +1775,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1723,7 +1789,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1749,7 +1814,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1838,6 +1902,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2409-452D-BC31-0A3DE54B2DB1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1873,7 +1942,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1907,7 +1975,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1949,7 +2016,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1979,7 +2052,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1996,20 +2075,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>666756</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>910596</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>403859</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2256,7 +2341,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2286,7 +2377,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2561,7 +2658,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2594,9 +2691,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2629,6 +2743,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2804,21 +2935,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R17" sqref="R17"/>
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O25" sqref="O25:Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2838,7 +2970,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2846,7 +2978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2854,7 +2986,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2880,7 +3012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2906,7 +3038,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2915,7 +3047,7 @@
         <v>67.75</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2937,7 +3069,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2981,7 +3113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>62</v>
       </c>
@@ -3026,7 +3158,7 @@
         <v>16.690000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>63</v>
       </c>
@@ -3071,7 +3203,7 @@
         <v>17.79</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>64</v>
       </c>
@@ -3116,7 +3248,7 @@
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>65</v>
       </c>
@@ -3161,7 +3293,7 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>66</v>
       </c>
@@ -3206,7 +3338,7 @@
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>67</v>
       </c>
@@ -3251,7 +3383,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>68</v>
       </c>
@@ -3296,7 +3428,7 @@
         <v>-1.29</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>69</v>
       </c>
@@ -3341,7 +3473,7 @@
         <v>-5.86</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
@@ -3386,7 +3518,7 @@
         <v>-10.63</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>71</v>
       </c>
@@ -3431,7 +3563,7 @@
         <v>-14.55</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>72</v>
       </c>
@@ -3476,7 +3608,7 @@
         <v>-17.03</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>73</v>
       </c>
@@ -3521,7 +3653,7 @@
         <v>-17.079999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>74</v>
       </c>
@@ -3566,7 +3698,7 @@
         <v>-15.32</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="2" t="s">
         <v>28</v>
       </c>
@@ -3589,7 +3721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>62</v>
       </c>
@@ -3638,7 +3770,7 @@
         <v>166.8</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>63</v>
       </c>
@@ -3691,7 +3823,7 @@
         <v>0.29499999999999815</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>64</v>
       </c>
@@ -3744,7 +3876,7 @@
         <v>2.7849999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>65</v>
       </c>
@@ -3797,7 +3929,7 @@
         <v>4.0500000000000025</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>66</v>
       </c>
@@ -3850,7 +3982,7 @@
         <v>4.3650000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>67</v>
       </c>
@@ -3903,7 +4035,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>68</v>
       </c>
@@ -3956,7 +4088,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>69</v>
       </c>
@@ -4009,7 +4141,7 @@
         <v>4.7050000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>70</v>
       </c>
@@ -4062,7 +4194,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>71</v>
       </c>
@@ -4115,7 +4247,7 @@
         <v>3.1950000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>72</v>
       </c>
@@ -4168,7 +4300,7 @@
         <v>1.1749999999999989</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>73</v>
       </c>
@@ -4221,7 +4353,7 @@
         <v>-1.1750000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>74</v>
       </c>
@@ -4272,6 +4404,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="K7:M7"/>
@@ -4279,9 +4414,6 @@
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4289,21 +4421,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T37" sqref="T37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O25" sqref="O25:Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4323,7 +4456,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4331,7 +4464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4339,7 +4472,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4365,7 +4498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4391,7 +4524,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4400,7 +4533,7 @@
         <v>67.75</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -4422,7 +4555,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4466,7 +4599,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>62</v>
       </c>
@@ -4511,7 +4644,7 @@
         <v>6.07</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>63</v>
       </c>
@@ -4556,7 +4689,7 @@
         <v>8.06</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>64</v>
       </c>
@@ -4601,7 +4734,7 @@
         <v>9.44</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>65</v>
       </c>
@@ -4646,7 +4779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>66</v>
       </c>
@@ -4691,7 +4824,7 @@
         <v>6.81</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>67</v>
       </c>
@@ -4736,7 +4869,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>68</v>
       </c>
@@ -4781,7 +4914,7 @@
         <v>-0.83</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>69</v>
       </c>
@@ -4826,7 +4959,7 @@
         <v>-4.16</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
@@ -4871,7 +5004,7 @@
         <v>-7.1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>71</v>
       </c>
@@ -4916,7 +5049,7 @@
         <v>-8.11</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>72</v>
       </c>
@@ -4961,7 +5094,7 @@
         <v>-7.51</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>73</v>
       </c>
@@ -5006,7 +5139,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>74</v>
       </c>
@@ -5051,7 +5184,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="2" t="s">
         <v>28</v>
       </c>
@@ -5071,7 +5204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>62</v>
       </c>
@@ -5116,7 +5249,7 @@
         <v>6.0600000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>63</v>
       </c>
@@ -5165,7 +5298,7 @@
         <v>-1.5249999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>64</v>
       </c>
@@ -5214,7 +5347,7 @@
         <v>-0.29999999999999982</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>65</v>
       </c>
@@ -5263,7 +5396,7 @@
         <v>1.4249999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>66</v>
       </c>
@@ -5312,7 +5445,7 @@
         <v>2.7350000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>67</v>
       </c>
@@ -5361,7 +5494,7 @@
         <v>3.6749999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>68</v>
       </c>
@@ -5410,7 +5543,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>69</v>
       </c>
@@ -5459,7 +5592,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>70</v>
       </c>
@@ -5508,7 +5641,7 @@
         <v>1.7899999999999991</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>71</v>
       </c>
@@ -5557,7 +5690,7 @@
         <v>0.20000000000000018</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>72</v>
       </c>
@@ -5606,7 +5739,7 @@
         <v>-1.0449999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>73</v>
       </c>
@@ -5655,7 +5788,7 @@
         <v>-1.625</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>74</v>
       </c>
@@ -5702,6 +5835,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="K7:M7"/>
@@ -5709,11 +5845,1277 @@
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2141C916-DC60-4D68-9659-CCC6667BBAE6}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>0.16</v>
+      </c>
+      <c r="C2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D2">
+        <v>-1.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="D3">
+        <v>-1.8599999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.34</v>
+      </c>
+      <c r="D4">
+        <v>-2.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>0.03</v>
+      </c>
+      <c r="C5">
+        <v>-0.14999999999999991</v>
+      </c>
+      <c r="D5">
+        <v>-3.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-5.0000000000000017E-2</v>
+      </c>
+      <c r="C6">
+        <v>-0.36999999999999994</v>
+      </c>
+      <c r="D6">
+        <v>-4.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="C7">
+        <v>-0.53</v>
+      </c>
+      <c r="D7">
+        <v>-5.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>0.06</v>
+      </c>
+      <c r="C8">
+        <v>-0.81</v>
+      </c>
+      <c r="D8">
+        <v>-7.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>1.999999999999999E-2</v>
+      </c>
+      <c r="C9">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="D9">
+        <v>-11.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="C10">
+        <v>-1.18</v>
+      </c>
+      <c r="D10">
+        <v>-14.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="C11">
+        <v>-0.78999999999999992</v>
+      </c>
+      <c r="D11">
+        <v>-17.259999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>0.89</v>
+      </c>
+      <c r="C12">
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="D12">
+        <v>-19.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>1.26</v>
+      </c>
+      <c r="C13">
+        <v>1.4300000000000002</v>
+      </c>
+      <c r="D13">
+        <v>-18.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>1.48</v>
+      </c>
+      <c r="C14">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="D14">
+        <v>-15.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15056345-FF0B-427F-93D6-5E044922BD8B}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>-0.65999999999999992</v>
+      </c>
+      <c r="C2">
+        <v>0.54</v>
+      </c>
+      <c r="D2">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>-1.01</v>
+      </c>
+      <c r="C3">
+        <v>-0.33999999999999997</v>
+      </c>
+      <c r="D3">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>-1.35</v>
+      </c>
+      <c r="C4">
+        <v>-1.38</v>
+      </c>
+      <c r="D4">
+        <v>18.170000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="C5">
+        <v>-1.8900000000000001</v>
+      </c>
+      <c r="D5">
+        <v>15.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-1.01</v>
+      </c>
+      <c r="C6">
+        <v>-1.8599999999999999</v>
+      </c>
+      <c r="D6">
+        <v>11.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>-0.82000000000000006</v>
+      </c>
+      <c r="C7">
+        <v>-1.52</v>
+      </c>
+      <c r="D7">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>-0.54</v>
+      </c>
+      <c r="C8">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="D8">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>-0.41</v>
+      </c>
+      <c r="C9">
+        <v>-1.05</v>
+      </c>
+      <c r="D9">
+        <v>4.2100000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="C10">
+        <v>-0.99</v>
+      </c>
+      <c r="D10">
+        <v>3.2399999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="C11">
+        <v>-0.85</v>
+      </c>
+      <c r="D11">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>-0.20999999999999996</v>
+      </c>
+      <c r="C12">
+        <v>-0.63</v>
+      </c>
+      <c r="D12">
+        <v>2.3600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>-0.23000000000000004</v>
+      </c>
+      <c r="C13">
+        <v>-0.25</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>-0.12</v>
+      </c>
+      <c r="C14">
+        <v>4.9999999999999933E-2</v>
+      </c>
+      <c r="D14">
+        <v>1.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501D407C-F588-4154-AB94-40E248F6A93A}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>-0.44</v>
+      </c>
+      <c r="C2">
+        <v>0.46</v>
+      </c>
+      <c r="D2">
+        <v>16.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>-0.53999999999999992</v>
+      </c>
+      <c r="C3">
+        <v>-0.35</v>
+      </c>
+      <c r="D3">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>-0.76</v>
+      </c>
+      <c r="C4">
+        <v>-1.45</v>
+      </c>
+      <c r="D4">
+        <v>16.090000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>-0.65</v>
+      </c>
+      <c r="C5">
+        <v>-2.0099999999999998</v>
+      </c>
+      <c r="D5">
+        <v>12.040000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-0.69</v>
+      </c>
+      <c r="C6">
+        <v>-2.0299999999999998</v>
+      </c>
+      <c r="D6">
+        <v>7.9899999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>-0.53</v>
+      </c>
+      <c r="C7">
+        <v>-1.7500000000000002</v>
+      </c>
+      <c r="D7">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>-0.39</v>
+      </c>
+      <c r="C8">
+        <v>-1.5799999999999998</v>
+      </c>
+      <c r="D8">
+        <v>-1.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>-0.34</v>
+      </c>
+      <c r="C9">
+        <v>-1.56</v>
+      </c>
+      <c r="D9">
+        <v>-6.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>-0.25</v>
+      </c>
+      <c r="C10">
+        <v>-1.44</v>
+      </c>
+      <c r="D10">
+        <v>-10.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>-3.999999999999998E-2</v>
+      </c>
+      <c r="C11">
+        <v>-0.91</v>
+      </c>
+      <c r="D11">
+        <v>-14.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>0.25</v>
+      </c>
+      <c r="C12">
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="D12">
+        <v>-17.350000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>0.62</v>
+      </c>
+      <c r="C13">
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="D13">
+        <v>-17.259999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>0.99</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>-15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6947A0-6767-4AC5-B78D-6C1A3FC9A973}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>3.9999999999999994E-2</v>
+      </c>
+      <c r="C2">
+        <v>-0.06</v>
+      </c>
+      <c r="D2">
+        <v>-1.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="C3">
+        <v>-7.999999999999996E-2</v>
+      </c>
+      <c r="D3">
+        <v>-1.6099999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>9.9999999999999811E-3</v>
+      </c>
+      <c r="C4">
+        <v>-0.17999999999999994</v>
+      </c>
+      <c r="D4">
+        <v>-1.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-0.26999999999999991</v>
+      </c>
+      <c r="D5">
+        <v>-2.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="C6">
+        <v>-0.37999999999999995</v>
+      </c>
+      <c r="D6">
+        <v>-3.6500000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>9.9999999999999811E-3</v>
+      </c>
+      <c r="C7">
+        <v>-0.48000000000000004</v>
+      </c>
+      <c r="D7">
+        <v>-4.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="C8">
+        <v>-0.64000000000000012</v>
+      </c>
+      <c r="D8">
+        <v>-6.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>0.16</v>
+      </c>
+      <c r="C9">
+        <v>-0.56999999999999984</v>
+      </c>
+      <c r="D9">
+        <v>-9.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>0.39</v>
+      </c>
+      <c r="C10">
+        <v>-6.9999999999999951E-2</v>
+      </c>
+      <c r="D10">
+        <v>-10.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>0.71</v>
+      </c>
+      <c r="C11">
+        <v>0.65</v>
+      </c>
+      <c r="D11">
+        <v>-10.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>0.69</v>
+      </c>
+      <c r="C12">
+        <v>1.17</v>
+      </c>
+      <c r="D12">
+        <v>-9.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C13">
+        <v>1.28</v>
+      </c>
+      <c r="D13">
+        <v>-7.79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+      <c r="C14">
+        <v>1.05</v>
+      </c>
+      <c r="D14">
+        <v>-0.27299999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30087A-7FAF-4479-8731-6520F3DF7CD9}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>-0.17</v>
+      </c>
+      <c r="C2">
+        <v>0.43000000000000005</v>
+      </c>
+      <c r="D2">
+        <v>7.1800000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>-0.14999999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.38</v>
+      </c>
+      <c r="D3">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>-0.42</v>
+      </c>
+      <c r="C4">
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="D4">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>-0.49</v>
+      </c>
+      <c r="C5">
+        <v>-0.60999999999999988</v>
+      </c>
+      <c r="D5">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-0.57000000000000006</v>
+      </c>
+      <c r="C6">
+        <v>-1.03</v>
+      </c>
+      <c r="D6">
+        <v>9.879999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>-0.53</v>
+      </c>
+      <c r="C7">
+        <v>-1.1400000000000001</v>
+      </c>
+      <c r="D7">
+        <v>7.9099999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>-0.37</v>
+      </c>
+      <c r="C8">
+        <v>-1.02</v>
+      </c>
+      <c r="D8">
+        <v>5.7200000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>-0.35000000000000003</v>
+      </c>
+      <c r="C9">
+        <v>-0.87999999999999989</v>
+      </c>
+      <c r="D9">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>-0.26</v>
+      </c>
+      <c r="C10">
+        <v>-0.65999999999999992</v>
+      </c>
+      <c r="D10">
+        <v>3.2199999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="C11">
+        <v>-0.4</v>
+      </c>
+      <c r="D11">
+        <v>2.5500000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="C12">
+        <v>2.81</v>
+      </c>
+      <c r="D12">
+        <v>1.8800000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="C13">
+        <v>-6.0000000000000053E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.3800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="C14">
+        <v>2.9999999999999916E-2</v>
+      </c>
+      <c r="D14">
+        <v>1.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81064E18-45B2-4F07-9265-D00E2EE285BE}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.75</v>
+      </c>
+      <c r="B2">
+        <v>-0.06</v>
+      </c>
+      <c r="C2">
+        <v>0.38</v>
+      </c>
+      <c r="D2">
+        <v>6.0600000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.75</v>
+      </c>
+      <c r="B3">
+        <v>-0.10999999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.26</v>
+      </c>
+      <c r="D3">
+        <v>7.8800000000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.75</v>
+      </c>
+      <c r="B4">
+        <v>-0.32</v>
+      </c>
+      <c r="C4">
+        <v>-0.22999999999999998</v>
+      </c>
+      <c r="D4">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.75</v>
+      </c>
+      <c r="B5">
+        <v>-0.44000000000000006</v>
+      </c>
+      <c r="C5">
+        <v>-0.77</v>
+      </c>
+      <c r="D5">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.75</v>
+      </c>
+      <c r="B6">
+        <v>-0.42000000000000004</v>
+      </c>
+      <c r="C6">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="D6">
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>-0.33</v>
+      </c>
+      <c r="C7">
+        <v>-1.31</v>
+      </c>
+      <c r="D7">
+        <v>3.0100000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.25</v>
+      </c>
+      <c r="B8">
+        <v>-0.25</v>
+      </c>
+      <c r="C8">
+        <v>-1.28</v>
+      </c>
+      <c r="D8">
+        <v>-1.0899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1.25</v>
+      </c>
+      <c r="B9">
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="C9">
+        <v>-1.03</v>
+      </c>
+      <c r="D9">
+        <v>-4.8900000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-2.25</v>
+      </c>
+      <c r="B10">
+        <v>0.09</v>
+      </c>
+      <c r="C10">
+        <v>-0.43999999999999995</v>
+      </c>
+      <c r="D10">
+        <v>-7.43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-3.25</v>
+      </c>
+      <c r="B11">
+        <v>0.43000000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11">
+        <v>-8.4699999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-4.25</v>
+      </c>
+      <c r="B12">
+        <v>0.65</v>
+      </c>
+      <c r="C12">
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="D12">
+        <v>-7.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5.25</v>
+      </c>
+      <c r="B13">
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="C13">
+        <v>0.98</v>
+      </c>
+      <c r="D13">
+        <v>-6.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-6.25</v>
+      </c>
+      <c r="B14">
+        <v>0.61</v>
+      </c>
+      <c r="C14">
+        <v>0.85</v>
+      </c>
+      <c r="D14">
+        <v>-4.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>